<commit_message>
Added one more attempt to the cutadapt log; created adapter files without OR sequences; added QC for the second attempt.
</commit_message>
<xml_diff>
--- a/02_trimming/overrepresented.xlsx
+++ b/02_trimming/overrepresented.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mb62095\rnaseq_2021\02_trimming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{7A1DED49-03ED-4A5A-8AC4-AA4B465F8784}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD775CD5-625D-4BF6-B63D-08F513BB60A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" activeTab="2" xr2:uid="{056CAB12-26C1-4F8D-9DA5-EDBFE8581F18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" activeTab="1" xr2:uid="{056CAB12-26C1-4F8D-9DA5-EDBFE8581F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="170">
   <si>
     <t>GTTTAATGAGGCTCTGGACCGAGTTGGGCTTGCAATGCAGCGGCCTGTTA</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>&gt;OR15</t>
+  </si>
+  <si>
+    <t>CTTGGTACCGTGTCTTTGCCTGGGTCCATGGTGTGCCTTTGTTGGCCTGC</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +940,7 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,108 +949,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>2</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>1</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1064,13 +1067,13 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
@@ -1094,7 +1097,7 @@
       <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="P4" t="s">
@@ -1114,13 +1117,13 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H5" t="s">
@@ -1170,7 +1173,7 @@
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
@@ -2496,6 +2499,9 @@
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>169</v>
+      </c>
       <c r="F39" t="s">
         <v>64</v>
       </c>
@@ -2582,16 +2588,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2602,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31C65A6-4644-419E-9725-32AD19D05C5A}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K29" activeCellId="1" sqref="A31:A37 K29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BB82DD-E67F-4798-86BC-E2E8CCD7B9FB}">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A1:A30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed the OR sequences.
</commit_message>
<xml_diff>
--- a/02_trimming/overrepresented.xlsx
+++ b/02_trimming/overrepresented.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mb62095\rnaseq_2021\02_trimming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD775CD5-625D-4BF6-B63D-08F513BB60A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA855CB-9494-4883-8DE9-ECCBAF7CC1D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" activeTab="1" xr2:uid="{056CAB12-26C1-4F8D-9DA5-EDBFE8581F18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9330" xr2:uid="{056CAB12-26C1-4F8D-9DA5-EDBFE8581F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="236">
   <si>
     <t>GTTTAATGAGGCTCTGGACCGAGTTGGGCTTGCAATGCAGCGGCCTGTTA</t>
   </si>
@@ -537,6 +537,204 @@
   </si>
   <si>
     <t>CTTGGTACCGTGTCTTTGCCTGGGTCCATGGTGTGCCTTTGTTGGCCTGC</t>
+  </si>
+  <si>
+    <t>&gt;OR16</t>
+  </si>
+  <si>
+    <t>&gt;OR17</t>
+  </si>
+  <si>
+    <t>&gt;OR18</t>
+  </si>
+  <si>
+    <t>&gt;OR19</t>
+  </si>
+  <si>
+    <t>&gt;OR20</t>
+  </si>
+  <si>
+    <t>&gt;OR21</t>
+  </si>
+  <si>
+    <t>&gt;OR22</t>
+  </si>
+  <si>
+    <t>&gt;OR23</t>
+  </si>
+  <si>
+    <t>&gt;OR24</t>
+  </si>
+  <si>
+    <t>&gt;OR25</t>
+  </si>
+  <si>
+    <t>&gt;OR26</t>
+  </si>
+  <si>
+    <t>&gt;OR27</t>
+  </si>
+  <si>
+    <t>&gt;OR28</t>
+  </si>
+  <si>
+    <t>&gt;OR29</t>
+  </si>
+  <si>
+    <t>&gt;OR30</t>
+  </si>
+  <si>
+    <t>&gt;OR31</t>
+  </si>
+  <si>
+    <t>&gt;OR32</t>
+  </si>
+  <si>
+    <t>&gt;OR33</t>
+  </si>
+  <si>
+    <t>&gt;OR34</t>
+  </si>
+  <si>
+    <t>&gt;OR35</t>
+  </si>
+  <si>
+    <t>&gt;OR36</t>
+  </si>
+  <si>
+    <t>&gt;OR37</t>
+  </si>
+  <si>
+    <t>&gt;OR38</t>
+  </si>
+  <si>
+    <t>&gt;OR39</t>
+  </si>
+  <si>
+    <t>&gt;OR40</t>
+  </si>
+  <si>
+    <t>&gt;OR41</t>
+  </si>
+  <si>
+    <t>&gt;OR42</t>
+  </si>
+  <si>
+    <t>&gt;OR43</t>
+  </si>
+  <si>
+    <t>&gt;OR44</t>
+  </si>
+  <si>
+    <t>&gt;OR45</t>
+  </si>
+  <si>
+    <t>&gt;OR46</t>
+  </si>
+  <si>
+    <t>&gt;OR47</t>
+  </si>
+  <si>
+    <t>&gt;OR48</t>
+  </si>
+  <si>
+    <t>&gt;OR49</t>
+  </si>
+  <si>
+    <t>&gt;OR50</t>
+  </si>
+  <si>
+    <t>&gt;OR51</t>
+  </si>
+  <si>
+    <t>&gt;OR52</t>
+  </si>
+  <si>
+    <t>&gt;OR53</t>
+  </si>
+  <si>
+    <t>&gt;OR54</t>
+  </si>
+  <si>
+    <t>&gt;OR55</t>
+  </si>
+  <si>
+    <t>&gt;OR56</t>
+  </si>
+  <si>
+    <t>&gt;OR57</t>
+  </si>
+  <si>
+    <t>&gt;OR58</t>
+  </si>
+  <si>
+    <t>&gt;OR59</t>
+  </si>
+  <si>
+    <t>&gt;OR60</t>
+  </si>
+  <si>
+    <t>CTGTTGTAGTATGAGTCTGGGCCTTAAGTGAGCCCATGCTGCAGTG</t>
+  </si>
+  <si>
+    <t>&gt;OR61</t>
+  </si>
+  <si>
+    <t>&gt;OR62</t>
+  </si>
+  <si>
+    <t>CTGCTTTAGTATGAAGTCTAGGCCTTAAAGCGAGCCCATGCTGCAGTG</t>
+  </si>
+  <si>
+    <t>&gt;OR63</t>
+  </si>
+  <si>
+    <t>&gt;OR64</t>
+  </si>
+  <si>
+    <t>&gt;OR65</t>
+  </si>
+  <si>
+    <t>&gt;OR66</t>
+  </si>
+  <si>
+    <t>&gt;OR67</t>
+  </si>
+  <si>
+    <t>GTTGTAGTATGAGTCTGGGCCTTAAGTGAGCCCATGCTGCAGTG</t>
+  </si>
+  <si>
+    <t>&gt;OR68</t>
+  </si>
+  <si>
+    <t>&gt;OR69</t>
+  </si>
+  <si>
+    <t>GTCTGTTGTAGTATGAGTCTGGGCCTTAAGTGAGCCCATGCTGCAGTG</t>
+  </si>
+  <si>
+    <t>&gt;OR70</t>
+  </si>
+  <si>
+    <t>&gt;OR71</t>
+  </si>
+  <si>
+    <t>&gt;OR72</t>
+  </si>
+  <si>
+    <t>&gt;OR73</t>
+  </si>
+  <si>
+    <t>&gt;OR74</t>
+  </si>
+  <si>
+    <t>AGCGGATGGGGGCTGGCGACGCGCACCGGCCGTATGCGGAACGGCTCCTG</t>
+  </si>
+  <si>
+    <t>&gt;OR75</t>
+  </si>
+  <si>
+    <t>GAAAGGGAATCGGGTTAAGATTTCCCGAGCCGGGACGTGGCGGCAGACGG</t>
   </si>
 </sst>
 </file>
@@ -616,7 +814,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -937,18 +1145,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E87D600-548F-4B28-B1E8-788B776DDE6E}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:Z151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z2" activeCellId="1" sqref="A4:P49 Z2:Z151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="16" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -970,7 +1179,7 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1003,8 +1212,11 @@
         <v>26</v>
       </c>
       <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1053,8 +1265,11 @@
       <c r="P3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1103,8 +1318,11 @@
       <c r="P4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1371,11 @@
       <c r="P5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1203,8 +1424,11 @@
       <c r="P6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1253,8 +1477,11 @@
       <c r="P7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1303,8 +1530,11 @@
       <c r="P8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1353,8 +1583,11 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1403,8 +1636,11 @@
       <c r="P10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1453,8 +1689,11 @@
       <c r="P11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1503,8 +1742,11 @@
       <c r="P12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1553,8 +1795,11 @@
       <c r="P13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1603,8 +1848,11 @@
       <c r="P14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1653,8 +1901,11 @@
       <c r="P15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1703,8 +1954,11 @@
       <c r="P16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1753,8 +2007,11 @@
       <c r="P17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -1803,8 +2060,11 @@
       <c r="P18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -1853,8 +2113,11 @@
       <c r="P19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1903,8 +2166,11 @@
       <c r="P20" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1953,8 +2219,11 @@
       <c r="P21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2003,8 +2272,11 @@
       <c r="P22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2053,8 +2325,11 @@
       <c r="P23" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2103,8 +2378,11 @@
       <c r="P24" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -2150,8 +2428,11 @@
       <c r="P25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2191,8 +2472,11 @@
       <c r="P26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -2226,8 +2510,11 @@
       <c r="P27" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -2261,8 +2548,11 @@
       <c r="P28" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -2293,8 +2583,11 @@
       <c r="P29" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2325,8 +2618,11 @@
       <c r="P30" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>57</v>
       </c>
@@ -2354,8 +2650,11 @@
       <c r="P31" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Z31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>49</v>
       </c>
@@ -2380,8 +2679,11 @@
       <c r="P32" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>133</v>
       </c>
@@ -2406,8 +2708,11 @@
       <c r="P33" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>59</v>
       </c>
@@ -2429,8 +2734,11 @@
       <c r="P34" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>60</v>
       </c>
@@ -2449,8 +2757,11 @@
       <c r="P35" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>61</v>
       </c>
@@ -2469,8 +2780,11 @@
       <c r="P36" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>62</v>
       </c>
@@ -2483,8 +2797,11 @@
       <c r="J37" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>63</v>
       </c>
@@ -2497,8 +2814,11 @@
       <c r="J38" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>169</v>
       </c>
@@ -2511,94 +2831,640 @@
       <c r="J39" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>109</v>
       </c>
       <c r="J40" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>110</v>
       </c>
       <c r="J41" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
         <v>45</v>
       </c>
       <c r="J42" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
         <v>62</v>
       </c>
       <c r="J43" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
         <v>56</v>
       </c>
       <c r="J44" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
         <v>111</v>
       </c>
       <c r="J45" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>112</v>
       </c>
       <c r="J46" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
         <v>113</v>
       </c>
       <c r="J47" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Z47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H48" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="Z48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
         <v>58</v>
       </c>
+      <c r="Z49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z50" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z62" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="Z64" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z66" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z68" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z72" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z75" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z76" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z78" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z79" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z80" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z82" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z83" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z84" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z86" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z87" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z88" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z90" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z91" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z92" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z94" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="95" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z95" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z96" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z98" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="99" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z100" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="101" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z102" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="103" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z103" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z104" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="105" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z106" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z108" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z110" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="111" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z111" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z112" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="113" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z113" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="114" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z114" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="115" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z115" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z116" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z117" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="118" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z118" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="119" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z119" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z121" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="122" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z122" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="123" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z123" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="124" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z124" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="125" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z125" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="126" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z126" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="127" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z127" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z128" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="129" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z130" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="131" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z132" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="133" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z133" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z134" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="135" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z135" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="136" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z136" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="137" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z137" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="138" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z138" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z139" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="140" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z140" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="141" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z141" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="142" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z142" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="143" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z143" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="144" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z144" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="145" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z145" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="146" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z146" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="147" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z147" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z148" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="149" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z149" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="150" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z150" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="151" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z151" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A4:P49 Z2:Z151">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2608,7 +3474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31C65A6-4644-419E-9725-32AD19D05C5A}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
@@ -3075,7 +3941,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A22 C2:C27">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>